<commit_message>
Spezpreis Kiosk - Einkaufspreis gelöscht
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub 2024\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7739464E-DF7D-4D57-8203-5FBB664C677B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DFEDC5-A493-4001-8468-373F5A649E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3084" yWindow="3780" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Verkaufspreis</t>
-  </si>
-  <si>
-    <t>Einkaufspreis</t>
   </si>
   <si>
     <t>Anzahl verkaufter Artikel</t>
@@ -127,10 +124,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     </dxf>
@@ -151,14 +145,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2E4FAC83-4FC6-4E6F-87B3-8377FC66120C}" name="Datum" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2E4FAC83-4FC6-4E6F-87B3-8377FC66120C}" name="Datum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{7C6D28F5-89B2-4342-9089-E87764A5F47F}" name="Spezialpreis"/>
     <tableColumn id="3" xr3:uid="{7FEC0B3F-B7F7-492A-A2CC-4C43E7370E3F}" name="Artikelname"/>
-    <tableColumn id="4" xr3:uid="{3EC8A94D-5F55-472D-905C-204DD835F9D2}" name="Verkaufspreis" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{966EAAE9-A0F8-4F52-B2B1-4534CD873A27}" name="Einkaufspreis" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3EC8A94D-5F55-472D-905C-204DD835F9D2}" name="Verkaufspreis" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{6D1A3E3C-8B9B-44F2-91C7-2874FB9B2AA1}" name="Anzahl verkaufter Artikel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -462,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,11 +467,10 @@
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,127 +486,106 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45311</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="E2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45311</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="E3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45311</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45311</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45312</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
-        <v>48.5</v>
-      </c>
-      <c r="F6">
+      <c r="E6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45312</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2">
         <v>50</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="E7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Einnahmen Old Oak Spez preise
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2063D4D5-2FF9-4A5C-9E46-7BA0C1F8AD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27E3D61-5DA6-4DC1-AADF-594C53714AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="5028" yWindow="3852" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Kaffee und Gipfeli</t>
+  </si>
+  <si>
+    <t>Kaffee und Gebäck</t>
+  </si>
+  <si>
+    <t>Gebäck</t>
+  </si>
+  <si>
+    <t>Kollekte</t>
   </si>
 </sst>
 </file>
@@ -154,8 +163,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2E4FAC83-4FC6-4E6F-87B3-8377FC66120C}" name="Datum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{7C6D28F5-89B2-4342-9089-E87764A5F47F}" name="Spezialpreis"/>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,6 +641,57 @@
         <v>4</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2">
+        <v>240</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Eintritte und Kiosk für 1.4.24
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A861C9D-CE30-4D9D-B73A-D63E118E1840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA455936-52DA-4AF7-B647-FAD874B5B7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="4200" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="5028" yWindow="3852" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Gebäck</t>
+  </si>
+  <si>
+    <t>Leibniz Kekse Dschungel</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,6 +675,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>104.24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Spez preis 21.4.24 plus Ella 2. Vorstelung ohne Mindestabgaben
</commit_message>
<xml_diff>
--- a/Input/Spezialpreisekiosk.xlsx
+++ b/Input/Spezialpreisekiosk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C604E2B0-264B-47FD-AD07-83B19F68DADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6752C71F-8486-4A11-9324-D2A789CFD917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5724" yWindow="4548" windowWidth="15684" windowHeight="11832" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{5CFCAA73-5DB4-4EB4-81C9-1C9C0D98D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Leibniz Kekse Dschungel</t>
+  </si>
+  <si>
+    <t>Treppensitze</t>
   </si>
 </sst>
 </file>
@@ -163,8 +166,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0">
-  <autoFilter ref="A1:E12" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13" xr:uid="{9A44B4B4-A546-4A04-B7DF-39B4610A3FD4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2E4FAC83-4FC6-4E6F-87B3-8377FC66120C}" name="Datum" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{7C6D28F5-89B2-4342-9089-E87764A5F47F}" name="Spezialpreis"/>
@@ -473,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD21FE1F-65EF-43DF-AD1F-FCA81656A71F}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,6 +695,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45403</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>